<commit_message>
fixstation loading is working well... ish
</commit_message>
<xml_diff>
--- a/core/tests/sample_data/FilterLog.xlsx
+++ b/core/tests/sample_data/FilterLog.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Gov\Projects\djangoProject\dart\core\tests\sample_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{2620A38B-1E63-4F0E-A258-7D46F68AA674}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5C2C5BC-9B01-4D1A-A8EC-D07F1CD48682}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="21600" windowHeight="13176" activeTab="1" xr2:uid="{90BC93A9-37F2-43F3-8B40-765139D73F8A}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="25440" windowHeight="15990" activeTab="1" xr2:uid="{90BC93A9-37F2-43F3-8B40-765139D73F8A}"/>
   </bookViews>
   <sheets>
     <sheet name="HL_0" sheetId="3" r:id="rId1"/>
@@ -19,7 +19,6 @@
     <sheet name="Shediac Valley" sheetId="5" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -466,23 +465,23 @@
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.28515625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="9" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.88671875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.44140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.6640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="16.33203125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="14.5546875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="5.109375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="8.109375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="6.33203125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="7.6640625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="6.5546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="5.140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="8.140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="6.28515625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="7.7109375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="6.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="21" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:12" ht="21" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -520,7 +519,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B2">
         <v>60</v>
       </c>
@@ -551,7 +550,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B3">
         <v>10</v>
       </c>
@@ -576,7 +575,7 @@
       </c>
       <c r="L3" s="1"/>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B4">
         <v>5</v>
       </c>
@@ -607,7 +606,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B5">
         <v>1</v>
       </c>
@@ -646,26 +645,26 @@
   <dimension ref="A1:L57"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K1" sqref="K1"/>
+      <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="19.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.77734375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.6640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.6640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="6.88671875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="7.33203125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.88671875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11.6640625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="9.33203125" customWidth="1"/>
-    <col min="10" max="10" width="7.44140625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="9.33203125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="16.21875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="19.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="6.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="7.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9.28515625" customWidth="1"/>
+    <col min="10" max="10" width="7.42578125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="16.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="21" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:12" ht="21" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -703,299 +702,317 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" s="3">
-        <v>495271</v>
-      </c>
-      <c r="B2" s="3">
+        <v>496479</v>
+      </c>
+      <c r="B2">
         <v>140</v>
       </c>
-      <c r="C2" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="D2" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="E2" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="F2" s="3"/>
-      <c r="G2" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="H2" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="I2" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="J2" s="3"/>
-      <c r="K2" s="3"/>
-      <c r="L2" s="3"/>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="C2" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="J2" s="1"/>
+      <c r="K2" s="1"/>
+      <c r="L2" s="1"/>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" s="3">
-        <v>495272</v>
-      </c>
-      <c r="B3" s="3">
+        <v>496478</v>
+      </c>
+      <c r="B3">
         <v>100</v>
       </c>
-      <c r="C3" s="3"/>
-      <c r="D3" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="E3" s="3"/>
-      <c r="F3" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="G3" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="H3" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="I3" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="J3" s="3"/>
-      <c r="K3" s="3"/>
-      <c r="L3" s="3"/>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="C3" s="1"/>
+      <c r="D3" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E3" s="1"/>
+      <c r="F3" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="I3" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="J3" s="1"/>
+      <c r="K3" s="1"/>
+      <c r="L3" s="1"/>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" s="3">
-        <v>495273</v>
-      </c>
-      <c r="B4" s="3">
-        <v>80</v>
-      </c>
-      <c r="C4" s="3"/>
-      <c r="D4" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="E4" s="3"/>
-      <c r="F4" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="G4" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="H4" s="3"/>
-      <c r="I4" s="3"/>
-      <c r="J4" s="3"/>
-      <c r="K4" s="3"/>
-      <c r="L4" s="3"/>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
+        <v>496477</v>
+      </c>
+      <c r="B4">
+        <v>75</v>
+      </c>
+      <c r="C4" s="1"/>
+      <c r="D4" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E4" s="1"/>
+      <c r="F4" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="H4" s="1"/>
+      <c r="I4" s="1"/>
+      <c r="J4" s="1"/>
+      <c r="K4" s="1"/>
+      <c r="L4" s="1"/>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" s="3">
-        <v>495274</v>
-      </c>
-      <c r="B5" s="3">
-        <v>80</v>
-      </c>
-      <c r="C5" s="3"/>
-      <c r="D5" s="3"/>
-      <c r="E5" s="3"/>
-      <c r="F5" s="3"/>
-      <c r="G5" s="3"/>
-      <c r="H5" s="3"/>
-      <c r="I5" s="3"/>
-      <c r="J5" s="3"/>
-      <c r="K5" s="3"/>
-      <c r="L5" s="3"/>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
+        <v>496476</v>
+      </c>
+      <c r="B5">
+        <v>50</v>
+      </c>
+      <c r="C5" s="1"/>
+      <c r="D5" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E5" s="1"/>
+      <c r="F5" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="H5" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="I5" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="J5" s="1"/>
+      <c r="K5" s="1"/>
+      <c r="L5" s="1"/>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" s="3">
-        <v>495275</v>
-      </c>
-      <c r="B6" s="3">
-        <v>80</v>
-      </c>
-      <c r="C6" s="3"/>
-      <c r="D6" s="3"/>
-      <c r="E6" s="3"/>
-      <c r="F6" s="3"/>
-      <c r="G6" s="3"/>
-      <c r="H6" s="3"/>
-      <c r="I6" s="3"/>
-      <c r="J6" s="3"/>
-      <c r="K6" s="3"/>
-      <c r="L6" s="3"/>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
+        <v>496475</v>
+      </c>
+      <c r="B6">
+        <v>40</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="H6" s="1"/>
+      <c r="I6" s="1"/>
+      <c r="J6" s="1"/>
+      <c r="K6" s="1"/>
+      <c r="L6" s="1"/>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" s="4">
-        <v>495276</v>
-      </c>
-      <c r="B7" s="4">
-        <v>60</v>
-      </c>
-      <c r="C7" s="4"/>
-      <c r="D7" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="E7" s="4"/>
-      <c r="F7" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="G7" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="H7" s="4"/>
-      <c r="I7" s="4"/>
-      <c r="J7" s="4"/>
-      <c r="K7" s="4"/>
-      <c r="L7" s="4"/>
-    </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
+        <v>496474</v>
+      </c>
+      <c r="B7">
+        <v>30</v>
+      </c>
+      <c r="C7" s="1"/>
+      <c r="D7" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E7" s="1"/>
+      <c r="F7" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="H7" s="1"/>
+      <c r="I7" s="1"/>
+      <c r="J7" s="1"/>
+      <c r="K7" s="1"/>
+      <c r="L7" s="1"/>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" s="3">
-        <v>495277</v>
-      </c>
-      <c r="B8" s="3">
-        <v>50</v>
-      </c>
-      <c r="C8" s="3"/>
-      <c r="D8" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="E8" s="3"/>
-      <c r="F8" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="G8" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="H8" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="I8" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="J8" s="3"/>
-      <c r="K8" s="3"/>
-      <c r="L8" s="3"/>
-    </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
+        <v>496473</v>
+      </c>
+      <c r="B8">
+        <v>20</v>
+      </c>
+      <c r="C8" s="1"/>
+      <c r="D8" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E8" s="1"/>
+      <c r="F8" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="G8" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="H8" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="I8" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="J8" s="1"/>
+      <c r="K8" s="1"/>
+      <c r="L8" s="1"/>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" s="3">
-        <v>495278</v>
-      </c>
-      <c r="B9" s="3">
-        <v>40</v>
-      </c>
-      <c r="C9" s="3"/>
-      <c r="D9" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="E9" s="3"/>
-      <c r="F9" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="G9" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="H9" s="3"/>
-      <c r="I9" s="3"/>
-      <c r="J9" s="3"/>
-      <c r="K9" s="3"/>
-      <c r="L9" s="3"/>
-    </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
+        <v>496472</v>
+      </c>
+      <c r="B9">
+        <v>10</v>
+      </c>
+      <c r="C9" s="1"/>
+      <c r="D9" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E9" s="1"/>
+      <c r="F9" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="G9" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="H9" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="I9" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="J9" s="1"/>
+      <c r="K9" s="1"/>
+      <c r="L9" s="1"/>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" s="3">
-        <v>495279</v>
-      </c>
-      <c r="B10" s="3">
-        <v>40</v>
-      </c>
-      <c r="C10" s="3"/>
-      <c r="D10" s="3"/>
-      <c r="E10" s="3"/>
-      <c r="F10" s="3"/>
-      <c r="G10" s="3"/>
-      <c r="H10" s="3"/>
-      <c r="I10" s="3"/>
-      <c r="J10" s="3"/>
-      <c r="K10" s="3"/>
-      <c r="L10" s="3"/>
-    </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
+        <v>496471</v>
+      </c>
+      <c r="B10">
+        <v>5</v>
+      </c>
+      <c r="C10" s="1"/>
+      <c r="D10" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E10" s="1"/>
+      <c r="F10" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="G10" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="H10" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="I10" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="J10" s="1"/>
+      <c r="K10" s="1"/>
+      <c r="L10" s="1"/>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11" s="3">
-        <v>495280</v>
-      </c>
-      <c r="B11" s="3">
-        <v>40</v>
-      </c>
-      <c r="C11" s="3"/>
-      <c r="D11" s="3"/>
-      <c r="E11" s="3"/>
-      <c r="F11" s="3"/>
-      <c r="G11" s="3"/>
-      <c r="H11" s="3"/>
-      <c r="I11" s="3"/>
-      <c r="J11" s="3"/>
-      <c r="K11" s="3"/>
-      <c r="L11" s="3"/>
-    </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A12" s="3">
-        <v>495281</v>
-      </c>
-      <c r="B12" s="3">
-        <v>30</v>
-      </c>
+        <v>496470</v>
+      </c>
+      <c r="B11">
+        <v>1</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="G11" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="H11" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="I11" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="J11" s="1"/>
+      <c r="K11" s="1"/>
+      <c r="L11" s="1"/>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A12" s="3"/>
+      <c r="B12" s="3"/>
       <c r="C12" s="3"/>
-      <c r="D12" s="3" t="s">
-        <v>10</v>
-      </c>
+      <c r="D12" s="3"/>
       <c r="E12" s="3"/>
-      <c r="F12" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="G12" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="H12" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="I12" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="J12" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="K12" s="3" t="s">
-        <v>10</v>
-      </c>
+      <c r="F12" s="3"/>
+      <c r="G12" s="3"/>
+      <c r="H12" s="3"/>
+      <c r="I12" s="3"/>
+      <c r="J12" s="3"/>
+      <c r="K12" s="3"/>
       <c r="L12" s="3"/>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A13" s="3">
-        <v>495282</v>
-      </c>
-      <c r="B13" s="3">
-        <v>20</v>
-      </c>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A13" s="3"/>
+      <c r="B13" s="3"/>
       <c r="C13" s="3"/>
-      <c r="D13" s="3" t="s">
-        <v>10</v>
-      </c>
+      <c r="D13" s="3"/>
       <c r="E13" s="3"/>
-      <c r="F13" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="G13" s="3" t="s">
-        <v>10</v>
-      </c>
+      <c r="F13" s="3"/>
+      <c r="G13" s="3"/>
       <c r="H13" s="3"/>
       <c r="I13" s="3"/>
       <c r="J13" s="3"/>
       <c r="K13" s="3"/>
       <c r="L13" s="3"/>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A14" s="3">
-        <v>495283</v>
-      </c>
-      <c r="B14" s="3">
-        <v>20</v>
-      </c>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A14" s="3"/>
+      <c r="B14" s="3"/>
       <c r="C14" s="3"/>
       <c r="D14" s="3"/>
       <c r="E14" s="3"/>
@@ -1007,13 +1024,9 @@
       <c r="K14" s="3"/>
       <c r="L14" s="3"/>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A15" s="3">
-        <v>495284</v>
-      </c>
-      <c r="B15" s="3">
-        <v>20</v>
-      </c>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A15" s="3"/>
+      <c r="B15" s="3"/>
       <c r="C15" s="3"/>
       <c r="D15" s="3"/>
       <c r="E15" s="3"/>
@@ -1025,79 +1038,37 @@
       <c r="K15" s="3"/>
       <c r="L15" s="3"/>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A16" s="3">
-        <v>495285</v>
-      </c>
-      <c r="B16" s="3">
-        <v>10</v>
-      </c>
-      <c r="C16" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="D16" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="E16" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="F16" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="G16" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="H16" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="I16" s="3" t="s">
-        <v>10</v>
-      </c>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A16" s="3"/>
+      <c r="B16" s="3"/>
+      <c r="C16" s="3"/>
+      <c r="D16" s="3"/>
+      <c r="E16" s="3"/>
+      <c r="F16" s="3"/>
+      <c r="G16" s="3"/>
+      <c r="H16" s="3"/>
+      <c r="I16" s="3"/>
       <c r="J16" s="3"/>
       <c r="K16" s="3"/>
       <c r="L16" s="3"/>
     </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A17" s="3">
-        <v>495286</v>
-      </c>
-      <c r="B17" s="3">
-        <v>1</v>
-      </c>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A17" s="3"/>
+      <c r="B17" s="3"/>
       <c r="C17" s="3"/>
-      <c r="D17" s="3" t="s">
-        <v>10</v>
-      </c>
+      <c r="D17" s="3"/>
       <c r="E17" s="3"/>
-      <c r="F17" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="G17" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="H17" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="I17" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="J17" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="K17" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="L17" s="3" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A18" s="3">
-        <v>495287</v>
-      </c>
-      <c r="B18" s="3">
-        <v>1</v>
-      </c>
+      <c r="F17" s="3"/>
+      <c r="G17" s="3"/>
+      <c r="H17" s="3"/>
+      <c r="I17" s="3"/>
+      <c r="J17" s="3"/>
+      <c r="K17" s="3"/>
+      <c r="L17" s="3"/>
+    </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A18" s="3"/>
+      <c r="B18" s="3"/>
       <c r="C18" s="3"/>
       <c r="D18" s="3"/>
       <c r="E18" s="3"/>
@@ -1109,13 +1080,9 @@
       <c r="K18" s="3"/>
       <c r="L18" s="3"/>
     </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A19" s="3">
-        <v>495288</v>
-      </c>
-      <c r="B19" s="3">
-        <v>1</v>
-      </c>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A19" s="3"/>
+      <c r="B19" s="3"/>
       <c r="C19" s="3"/>
       <c r="D19" s="3"/>
       <c r="E19" s="3"/>
@@ -1127,13 +1094,9 @@
       <c r="K19" s="3"/>
       <c r="L19" s="3"/>
     </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A20" s="3">
-        <v>495289</v>
-      </c>
-      <c r="B20" s="3">
-        <v>1</v>
-      </c>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A20" s="3"/>
+      <c r="B20" s="3"/>
       <c r="C20" s="3"/>
       <c r="D20" s="3"/>
       <c r="E20" s="3"/>
@@ -1145,7 +1108,7 @@
       <c r="K20" s="3"/>
       <c r="L20" s="3"/>
     </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A21" s="1"/>
       <c r="B21" s="1"/>
       <c r="C21" s="1"/>
@@ -1158,7 +1121,7 @@
       <c r="K21" s="1"/>
       <c r="L21" s="1"/>
     </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A22" s="1"/>
       <c r="B22" s="1"/>
       <c r="C22" s="1"/>
@@ -1171,7 +1134,7 @@
       <c r="K22" s="1"/>
       <c r="L22" s="1"/>
     </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A23" s="1"/>
       <c r="B23" s="1"/>
       <c r="C23" s="1"/>
@@ -1184,7 +1147,7 @@
       <c r="K23" s="1"/>
       <c r="L23" s="1"/>
     </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A24" s="1"/>
       <c r="B24" s="1"/>
       <c r="C24" s="1"/>
@@ -1197,7 +1160,7 @@
       <c r="K24" s="1"/>
       <c r="L24" s="1"/>
     </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A25" s="1"/>
       <c r="B25" s="1"/>
       <c r="C25" s="1"/>
@@ -1210,7 +1173,7 @@
       <c r="K25" s="1"/>
       <c r="L25" s="1"/>
     </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A26" s="1"/>
       <c r="B26" s="1"/>
       <c r="C26" s="1"/>
@@ -1223,7 +1186,7 @@
       <c r="K26" s="1"/>
       <c r="L26" s="1"/>
     </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A27" s="1"/>
       <c r="B27" s="1"/>
       <c r="C27" s="1"/>
@@ -1236,7 +1199,7 @@
       <c r="K27" s="1"/>
       <c r="L27" s="1"/>
     </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A28" s="1"/>
       <c r="B28" s="1"/>
       <c r="C28" s="1"/>
@@ -1249,7 +1212,7 @@
       <c r="K28" s="1"/>
       <c r="L28" s="1"/>
     </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A29" s="1"/>
       <c r="B29" s="1"/>
       <c r="C29" s="1"/>
@@ -1262,7 +1225,7 @@
       <c r="K29" s="1"/>
       <c r="L29" s="1"/>
     </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A30" s="1"/>
       <c r="B30" s="1"/>
       <c r="C30" s="1"/>
@@ -1275,7 +1238,7 @@
       <c r="K30" s="1"/>
       <c r="L30" s="1"/>
     </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A31" s="1"/>
       <c r="B31" s="1"/>
       <c r="C31" s="1"/>
@@ -1288,7 +1251,7 @@
       <c r="K31" s="1"/>
       <c r="L31" s="1"/>
     </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A32" s="1"/>
       <c r="B32" s="1"/>
       <c r="C32" s="1"/>
@@ -1301,7 +1264,7 @@
       <c r="K32" s="1"/>
       <c r="L32" s="1"/>
     </row>
-    <row r="33" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A33" s="1"/>
       <c r="B33" s="1"/>
       <c r="C33" s="1"/>
@@ -1314,7 +1277,7 @@
       <c r="K33" s="1"/>
       <c r="L33" s="1"/>
     </row>
-    <row r="34" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A34" s="1"/>
       <c r="B34" s="1"/>
       <c r="C34" s="1"/>
@@ -1327,7 +1290,7 @@
       <c r="K34" s="1"/>
       <c r="L34" s="1"/>
     </row>
-    <row r="35" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A35" s="1"/>
       <c r="B35" s="1"/>
       <c r="C35" s="1"/>
@@ -1340,7 +1303,7 @@
       <c r="K35" s="1"/>
       <c r="L35" s="1"/>
     </row>
-    <row r="36" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A36" s="1"/>
       <c r="B36" s="1"/>
       <c r="C36" s="1"/>
@@ -1353,7 +1316,7 @@
       <c r="K36" s="1"/>
       <c r="L36" s="1"/>
     </row>
-    <row r="37" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A37" s="1"/>
       <c r="B37" s="1"/>
       <c r="C37" s="1"/>
@@ -1366,7 +1329,7 @@
       <c r="K37" s="1"/>
       <c r="L37" s="1"/>
     </row>
-    <row r="38" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A38" s="1"/>
       <c r="B38" s="1"/>
       <c r="C38" s="1"/>
@@ -1379,7 +1342,7 @@
       <c r="K38" s="1"/>
       <c r="L38" s="1"/>
     </row>
-    <row r="39" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A39" s="1"/>
       <c r="B39" s="1"/>
       <c r="C39" s="1"/>
@@ -1392,7 +1355,7 @@
       <c r="K39" s="1"/>
       <c r="L39" s="1"/>
     </row>
-    <row r="40" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A40" s="1"/>
       <c r="B40" s="1"/>
       <c r="C40" s="1"/>
@@ -1405,7 +1368,7 @@
       <c r="K40" s="1"/>
       <c r="L40" s="1"/>
     </row>
-    <row r="41" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A41" s="1"/>
       <c r="B41" s="1"/>
       <c r="C41" s="1"/>
@@ -1418,7 +1381,7 @@
       <c r="K41" s="1"/>
       <c r="L41" s="1"/>
     </row>
-    <row r="42" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A42" s="1"/>
       <c r="B42" s="1"/>
       <c r="C42" s="1"/>
@@ -1431,7 +1394,7 @@
       <c r="K42" s="1"/>
       <c r="L42" s="1"/>
     </row>
-    <row r="43" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A43" s="1"/>
       <c r="B43" s="1"/>
       <c r="C43" s="1"/>
@@ -1444,7 +1407,7 @@
       <c r="K43" s="1"/>
       <c r="L43" s="1"/>
     </row>
-    <row r="44" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A44" s="1"/>
       <c r="B44" s="1"/>
       <c r="C44" s="1"/>
@@ -1457,7 +1420,7 @@
       <c r="K44" s="1"/>
       <c r="L44" s="1"/>
     </row>
-    <row r="45" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A45" s="1"/>
       <c r="B45" s="1"/>
       <c r="C45" s="1"/>
@@ -1470,7 +1433,7 @@
       <c r="K45" s="1"/>
       <c r="L45" s="1"/>
     </row>
-    <row r="46" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A46" s="1"/>
       <c r="B46" s="1"/>
       <c r="C46" s="1"/>
@@ -1483,7 +1446,7 @@
       <c r="K46" s="1"/>
       <c r="L46" s="1"/>
     </row>
-    <row r="47" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A47" s="1"/>
       <c r="B47" s="1"/>
       <c r="C47" s="1"/>
@@ -1496,7 +1459,7 @@
       <c r="K47" s="1"/>
       <c r="L47" s="1"/>
     </row>
-    <row r="48" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A48" s="1"/>
       <c r="B48" s="1"/>
       <c r="C48" s="1"/>
@@ -1509,7 +1472,7 @@
       <c r="K48" s="1"/>
       <c r="L48" s="1"/>
     </row>
-    <row r="49" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A49" s="1"/>
       <c r="B49" s="1"/>
       <c r="C49" s="1"/>
@@ -1522,7 +1485,7 @@
       <c r="K49" s="1"/>
       <c r="L49" s="1"/>
     </row>
-    <row r="50" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A50" s="1"/>
       <c r="B50" s="1"/>
       <c r="C50" s="1"/>
@@ -1535,7 +1498,7 @@
       <c r="K50" s="1"/>
       <c r="L50" s="1"/>
     </row>
-    <row r="51" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A51" s="1"/>
       <c r="B51" s="1"/>
       <c r="C51" s="1"/>
@@ -1548,7 +1511,7 @@
       <c r="K51" s="1"/>
       <c r="L51" s="1"/>
     </row>
-    <row r="52" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A52" s="1"/>
       <c r="B52" s="1"/>
       <c r="C52" s="1"/>
@@ -1561,7 +1524,7 @@
       <c r="K52" s="1"/>
       <c r="L52" s="1"/>
     </row>
-    <row r="53" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A53" s="1"/>
       <c r="B53" s="1"/>
       <c r="C53" s="1"/>
@@ -1574,7 +1537,7 @@
       <c r="K53" s="1"/>
       <c r="L53" s="1"/>
     </row>
-    <row r="54" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A54" s="1"/>
       <c r="B54" s="1"/>
       <c r="C54" s="1"/>
@@ -1587,7 +1550,7 @@
       <c r="K54" s="1"/>
       <c r="L54" s="1"/>
     </row>
-    <row r="55" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A55" s="1"/>
       <c r="B55" s="1"/>
       <c r="C55" s="1"/>
@@ -1600,7 +1563,7 @@
       <c r="K55" s="1"/>
       <c r="L55" s="1"/>
     </row>
-    <row r="56" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A56" s="1"/>
       <c r="B56" s="1"/>
       <c r="C56" s="1"/>
@@ -1613,7 +1576,7 @@
       <c r="K56" s="1"/>
       <c r="L56" s="1"/>
     </row>
-    <row r="57" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A57" s="1"/>
       <c r="B57" s="1"/>
       <c r="C57" s="1"/>
@@ -1640,23 +1603,23 @@
       <selection sqref="A1:L1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.28515625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="9" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.88671875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.44140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.6640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="16.33203125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="14.5546875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="5.109375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="8.109375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="6.33203125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="7.6640625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="6.5546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="5.140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="8.140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="6.28515625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="7.7109375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="6.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="21" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:12" ht="21" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1694,7 +1657,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B2">
         <v>90</v>
       </c>
@@ -1717,7 +1680,7 @@
       <c r="K2" s="1"/>
       <c r="L2" s="1"/>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B3">
         <v>50</v>
       </c>
@@ -1738,7 +1701,7 @@
       <c r="K3" s="1"/>
       <c r="L3" s="1"/>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B4">
         <v>25</v>
       </c>
@@ -1759,7 +1722,7 @@
       <c r="K4" s="1"/>
       <c r="L4" s="1"/>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B5">
         <v>10</v>
       </c>
@@ -1782,7 +1745,7 @@
       <c r="K5" s="1"/>
       <c r="L5" s="1"/>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B6">
         <v>1</v>
       </c>
@@ -1805,7 +1768,7 @@
       <c r="K6" s="1"/>
       <c r="L6" s="1"/>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="C7" s="1"/>
       <c r="D7" s="1"/>
       <c r="E7" s="1"/>
@@ -1817,7 +1780,7 @@
       <c r="K7" s="1"/>
       <c r="L7" s="1"/>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="C8" s="1"/>
       <c r="D8" s="1"/>
       <c r="E8" s="1"/>
@@ -1829,7 +1792,7 @@
       <c r="K8" s="1"/>
       <c r="L8" s="1"/>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="C9" s="1"/>
       <c r="D9" s="1"/>
       <c r="E9" s="1"/>
@@ -1841,7 +1804,7 @@
       <c r="K9" s="1"/>
       <c r="L9" s="1"/>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="C10" s="1"/>
       <c r="D10" s="1"/>
       <c r="E10" s="1"/>
@@ -1853,7 +1816,7 @@
       <c r="K10" s="1"/>
       <c r="L10" s="1"/>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="C11" s="1"/>
       <c r="D11" s="1"/>
       <c r="E11" s="1"/>
@@ -1878,23 +1841,23 @@
       <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.88671875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.6640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.88671875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.33203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.6640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15.88671875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="5.109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="5.140625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="8" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="6.33203125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="7.5546875" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="6.44140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="6.28515625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="7.5703125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="6.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="21" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:12" ht="21" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1932,7 +1895,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B2">
         <v>80</v>
       </c>
@@ -1957,7 +1920,7 @@
       <c r="K2" s="1"/>
       <c r="L2" s="1"/>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B3">
         <v>70</v>
       </c>
@@ -1978,7 +1941,7 @@
       <c r="K3" s="1"/>
       <c r="L3" s="1"/>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B4">
         <v>60</v>
       </c>
@@ -1999,7 +1962,7 @@
       <c r="K4" s="1"/>
       <c r="L4" s="1"/>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B5">
         <v>50</v>
       </c>
@@ -2024,7 +1987,7 @@
       <c r="K5" s="1"/>
       <c r="L5" s="1"/>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B6">
         <v>40</v>
       </c>
@@ -2045,7 +2008,7 @@
       <c r="K6" s="1"/>
       <c r="L6" s="1"/>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B7">
         <v>30</v>
       </c>
@@ -2061,7 +2024,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B8">
         <v>20</v>
       </c>
@@ -2081,7 +2044,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B9">
         <v>10</v>
       </c>
@@ -2097,7 +2060,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B10">
         <v>5</v>
       </c>
@@ -2113,7 +2076,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B11">
         <v>1</v>
       </c>
@@ -2133,7 +2096,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="D12" s="1"/>
     </row>
   </sheetData>

</xml_diff>